<commit_message>
- Loaded categories from firebase
</commit_message>
<xml_diff>
--- a/Document/Design.xlsx
+++ b/Document/Design.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Function</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>Design ask and answer screen (Bottle on doing)</t>
+  </si>
+  <si>
+    <t>Allow users to post messages that show up in their app.</t>
+  </si>
+  <si>
+    <t>Allow users to browse existing categories.</t>
+  </si>
+  <si>
+    <t>Allow users to create a new category, if the category they're looking for doesn't already exist.</t>
+  </si>
+  <si>
+    <t>Allow users to select a message to read more.</t>
+  </si>
+  <si>
+    <t>Allow users to comment on/reply to messages.</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -369,21 +387,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,8 +417,11 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -416,13 +437,45 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Fixed access query
</commit_message>
<xml_diff>
--- a/Document/Design.xlsx
+++ b/Document/Design.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Function</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Task to do</t>
   </si>
   <si>
-    <t>Add user and login function (Bottle on doing reskin login screen)</t>
-  </si>
-  <si>
-    <t>Design ask and answer screen (Bottle on doing)</t>
-  </si>
-  <si>
     <t>Allow users to post messages that show up in their app.</t>
   </si>
   <si>
@@ -70,17 +64,41 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Danh mục môn học</t>
+  </si>
+  <si>
+    <t>Show list categories</t>
+  </si>
+  <si>
+    <t>Add category</t>
+  </si>
+  <si>
+    <t>Add user and login function</t>
+  </si>
+  <si>
+    <t>Hà</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Design ask and answer screen</t>
+  </si>
+  <si>
+    <t>Bottle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -167,7 +185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -202,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -379,7 +397,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -387,21 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +438,11 @@
       <c r="F1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -435,43 +456,72 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>